<commit_message>
2.17 check available movement
</commit_message>
<xml_diff>
--- a/src/maps/main.xlsx
+++ b/src/maps/main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DKU\CompSci\201\Campus\src\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59136FE-98F9-4065-BD1A-0FA251186855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5443DD-7B82-4B8A-94CC-19C43A848795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -359,14 +359,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AN17" sqref="AN17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="3" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -378,6 +379,12 @@
       </c>
       <c r="C1">
         <v>32</v>
+      </c>
+      <c r="D1">
+        <v>5</v>
+      </c>
+      <c r="E1">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2.23 Tiles textures randomize
</commit_message>
<xml_diff>
--- a/src/maps/main.xlsx
+++ b/src/maps/main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DKU\CompSci\201\Campus\src\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5443DD-7B82-4B8A-94CC-19C43A848795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA252848-6A8A-497B-8DBD-B5AA60FBB055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -359,8 +359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG6" sqref="AG6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AN11" sqref="AN11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1601,13 +1601,13 @@
         <v>5</v>
       </c>
       <c r="M14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P14">
         <v>5</v>
@@ -1699,13 +1699,13 @@
         <v>5</v>
       </c>
       <c r="M15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P15">
         <v>5</v>

</xml_diff>